<commit_message>
Sync from main repo
</commit_message>
<xml_diff>
--- a/data/aip/Labels.xlsx
+++ b/data/aip/Labels.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{7E6B5C6F-2418-4D72-885A-0A459EF83910}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4C5A09C8-37F8-4FAD-A801-4FC32FF6D9EA}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{7E6B5C6F-2418-4D72-885A-0A459EF83910}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{98782E15-DEC5-40D4-93AE-5ECC9F90E156}"/>
   <bookViews>
-    <workbookView xWindow="372" yWindow="312" windowWidth="15654" windowHeight="10902" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2196" yWindow="642" windowWidth="15654" windowHeight="10902" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Labels" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Sync from customers and breaking changes
</commit_message>
<xml_diff>
--- a/data/aip/Labels.xlsx
+++ b/data/aip/Labels.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D84787-2972-4382-BF85-B595CD076234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFE9FD1-976A-4000-84F0-93BB44467798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11928" yWindow="1248" windowWidth="21852" windowHeight="11208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Labels" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="65">
   <si>
     <t>Internal.Internal</t>
   </si>
@@ -209,6 +209,12 @@
   </si>
   <si>
     <t>ALYAMG-ADM-AlleExternen@alyaconsulting031.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>SiteAndGroupProtection</t>
+  </si>
+  <si>
+    <t>AllowGuests</t>
   </si>
 </sst>
 </file>
@@ -546,7 +552,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -563,16 +569,17 @@
     <col min="4" max="4" width="23.109375" customWidth="1"/>
     <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" customWidth="1"/>
-    <col min="8" max="8" width="21.88671875" customWidth="1"/>
-    <col min="9" max="9" width="3" customWidth="1"/>
-    <col min="10" max="10" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="52.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
-    <col min="13" max="15" width="9" customWidth="1"/>
+    <col min="7" max="8" width="7.21875" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.88671875" customWidth="1"/>
+    <col min="11" max="11" width="3" customWidth="1"/>
+    <col min="12" max="12" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="15" max="17" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -592,34 +599,40 @@
         <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -635,17 +648,23 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N2" t="b">
-        <v>0</v>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
       </c>
       <c r="O2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -661,17 +680,23 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="M3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3" t="b">
-        <v>0</v>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
       </c>
       <c r="O3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -687,17 +712,23 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="M4" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" t="b">
-        <v>0</v>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
       </c>
       <c r="O4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -717,25 +748,31 @@
         <v>44</v>
       </c>
       <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>10</v>
       </c>
-      <c r="I5">
-        <v>7</v>
-      </c>
-      <c r="M5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" t="b">
-        <v>0</v>
+      <c r="K5">
+        <v>7</v>
       </c>
       <c r="O5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -755,25 +792,31 @@
         <v>44</v>
       </c>
       <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>10</v>
       </c>
-      <c r="I6">
-        <v>7</v>
-      </c>
-      <c r="M6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N6" t="b">
-        <v>0</v>
+      <c r="K6">
+        <v>7</v>
       </c>
       <c r="O6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -793,45 +836,51 @@
         <v>8</v>
       </c>
       <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" t="s">
         <v>9</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>10</v>
       </c>
-      <c r="I7">
-        <v>7</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="K7">
+        <v>7</v>
+      </c>
+      <c r="L7" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>11</v>
       </c>
-      <c r="M7" t="b">
-        <v>0</v>
-      </c>
-      <c r="N7" t="b">
-        <v>0</v>
-      </c>
       <c r="O7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="J8" t="s">
+      <c r="P7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -851,34 +900,40 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
         <v>9</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>10</v>
       </c>
-      <c r="I9">
-        <v>7</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="K9">
+        <v>7</v>
+      </c>
+      <c r="L9" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>11</v>
       </c>
-      <c r="M9" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" t="b">
-        <v>0</v>
-      </c>
       <c r="O9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -898,45 +953,51 @@
         <v>8</v>
       </c>
       <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>10</v>
       </c>
-      <c r="I10">
-        <v>7</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="K10">
+        <v>7</v>
+      </c>
+      <c r="L10" t="s">
         <v>59</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>11</v>
       </c>
-      <c r="M10" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" t="b">
-        <v>0</v>
-      </c>
       <c r="O10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="J11" t="s">
+      <c r="P10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L11" t="s">
         <v>61</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -956,38 +1017,44 @@
         <v>8</v>
       </c>
       <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
         <v>9</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>10</v>
       </c>
-      <c r="I12">
-        <v>7</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="K12">
+        <v>7</v>
+      </c>
+      <c r="L12" t="s">
         <v>59</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>11</v>
       </c>
-      <c r="M12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12" t="b">
-        <v>0</v>
-      </c>
       <c r="O12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K12" r:id="rId1" display="ALYAOG-ADM-AlleInternen@alyaconsulting031.onmicrosoft.com" xr:uid="{116AE952-8546-4BD0-AC68-11369981366D}"/>
-    <hyperlink ref="K11" r:id="rId2" display="ALYAOG-ADM-AlleExternen@alyaconsulting031.onmicrosoft.com" xr:uid="{1FB0CAF3-112C-49F0-A6FA-64CA85A5DEA9}"/>
-    <hyperlink ref="K8" r:id="rId3" display="ALYAOG-ADM-AlleExternen@alyaconsulting031.onmicrosoft.com" xr:uid="{208203AB-ED40-4DC4-866B-856EA4CE0920}"/>
+    <hyperlink ref="M12" r:id="rId1" display="ALYAOG-ADM-AlleInternen@alyaconsulting031.onmicrosoft.com" xr:uid="{116AE952-8546-4BD0-AC68-11369981366D}"/>
+    <hyperlink ref="M11" r:id="rId2" display="ALYAOG-ADM-AlleExternen@alyaconsulting031.onmicrosoft.com" xr:uid="{1FB0CAF3-112C-49F0-A6FA-64CA85A5DEA9}"/>
+    <hyperlink ref="M8" r:id="rId3" display="ALYAOG-ADM-AlleExternen@alyaconsulting031.onmicrosoft.com" xr:uid="{208203AB-ED40-4DC4-866B-856EA4CE0920}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>